<commit_message>
showing all available WoRMs images
</commit_message>
<xml_diff>
--- a/tnames.xlsx
+++ b/tnames.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Clupea harengus</t>
   </si>
@@ -151,13 +151,91 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -179,132 +257,132 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="2">
+      <c r="A2" t="s" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="2">
+      <c r="A3" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2">
+      <c r="A4" t="s" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="2">
+      <c r="A5" t="s" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="2">
+      <c r="A6" t="s" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="2">
+      <c r="A7" t="s" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="2">
+      <c r="A8" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="2">
+      <c r="A9" t="s" s="14">
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="2">
+      <c r="A10" t="s" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="2">
+      <c r="A11" t="s" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="2">
+      <c r="A12" t="s" s="17">
         <v>11</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="2">
+      <c r="A13" t="s" s="18">
         <v>12</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="2">
+      <c r="A14" t="s" s="19">
         <v>13</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="2">
+      <c r="A15" t="s" s="20">
         <v>14</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="2">
+      <c r="A16" t="s" s="21">
         <v>15</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="2">
+      <c r="A17" t="s" s="22">
         <v>16</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="2">
+      <c r="A18" t="s" s="23">
         <v>17</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="2">
+      <c r="A19" t="s" s="24">
         <v>18</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="2">
+      <c r="A20" t="s" s="25">
         <v>19</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="2">
+      <c r="A21" t="s" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="2">
+      <c r="A22" t="s" s="27">
         <v>21</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="2">
+      <c r="A23" t="s" s="28">
         <v>22</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="2">
+      <c r="A24" t="s" s="29">
         <v>23</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="2">
+      <c r="A25" t="s" s="30">
         <v>24</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="2">
+      <c r="A26" t="s" s="31">
         <v>25</v>
       </c>
     </row>

</xml_diff>